<commit_message>
fix laws page and contents
</commit_message>
<xml_diff>
--- a/lib/tasks/init/ley.xlsx
+++ b/lib/tasks/init/ley.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="171">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -484,15 +484,27 @@
 2. Dicho pronunciamiento permitirá continuar con la tramitación del procedimiento."</t>
   </si>
   <si>
+    <t xml:space="preserve">Artículo 49</t>
+  </si>
+  <si>
     <t xml:space="preserve">La Asamblea Legislativa de la Comunidad de Madrid y las entidades locales establecerán formas de participación ciudadana presenciales y electrónicas  en la elaboración de los Anteproyectos de ley y Reglamentos autonómicos y ordenanzas municipales que tengan como objeto cuestiones de especial relevancia en materia económica, social, ambiental, cultural, de género o territorial, para la región.</t>
   </si>
   <si>
+    <t xml:space="preserve">Artículo 50</t>
+  </si>
+  <si>
     <t xml:space="preserve">La participación ciudadana en la elaboración de normas y reglamentos se realizará a través de la participación de las personas residentes o de entidades de participación ciudadana cuyo ámbito de actuación, desde el punto de vista territorial o material, resulte afectado de forma directa por dicha norma o reglamento.</t>
   </si>
   <si>
+    <t xml:space="preserve">Artículo 51</t>
+  </si>
+  <si>
     <t xml:space="preserve">Las entidades de participación ciudadana o las personas residentes podrán solicitar la participación en el proceso de elaboración de un determinado anteproyecto de ley o reglamento, cuando consideren que incide de forma especial en su ámbito de actuación o de intereses y tengan el aval del 0,1 de la población censada en el ámbito territorial afectado por la norma. </t>
   </si>
   <si>
+    <t xml:space="preserve">Artículo 52</t>
+  </si>
+  <si>
     <t xml:space="preserve">La incorporación de las formas de participación ciudadana establecidas en este artículo se acomodarán al calendario legislativo o elaboración de reglamento cuyo cumplimiento haya comprometido el órgano correspondiente.</t>
   </si>
   <si>
@@ -502,10 +514,19 @@
     <t xml:space="preserve">Las entidades ciudadanas o las personas residentes podrán solicitar audiencia para mostrar su oposición a una norma o reglamento aprobado por las Cámara legislativa o Pleno Municipal, cuando consideren que les afecta directamente y de forma negativa.</t>
   </si>
   <si>
+    <t xml:space="preserve">Artículo 54</t>
+  </si>
+  <si>
     <t xml:space="preserve">Para iniciar un proceso de oposición popular se debe contar con el aval del 0,2 % del censo de la población.</t>
   </si>
   <si>
+    <t xml:space="preserve">Artículo 55</t>
+  </si>
+  <si>
     <t xml:space="preserve">El órgano competente deberá resolver de forma motivada sobre los efectos de la iniciativa de Oposición Popular.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Artículo 56</t>
   </si>
   <si>
     <t xml:space="preserve">Cuando una iniciativa de Oposición Popular alcance el aval del 0,5 % del censo de la población deberá tomarse en consideración la realización de una consulta popular. </t>
@@ -679,6 +700,9 @@
 2. Los convenios de colaboración establecerán las ayudas económicas para el desarrollo de una cultura de la participación y la realización de actividades participativas. Podrán tener un carácter plurianual.
 3. Se impulsarán planes de formación para los empleados públicos municipales en participación.
 4. Las entidades locales recibirán asistencia técnica para la realización de procesos participativo en su ámbito.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Artículo 76</t>
   </si>
   <si>
     <t xml:space="preserve">En los proyectos de intervención autonómica de iniciativa local, la Comunidad de Madrid, previa audiencia a la entidad local interesada, podrá solicitar la realización de un proceso participativo cuando la relevancia o características del proyecto lo aconsejen.</t>
@@ -910,13 +934,13 @@
   </sheetPr>
   <dimension ref="A1:Z80"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A48" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B77" activeCellId="0" sqref="B77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="16.3775510204082"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="18.3571428571429"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1797,13 +1821,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="n">
         <v>49</v>
       </c>
-      <c r="B50" s="1"/>
+      <c r="B50" s="1" t="s">
+        <v>104</v>
+      </c>
       <c r="C50" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>36</v>
@@ -1812,13 +1838,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="n">
         <v>50</v>
       </c>
-      <c r="B51" s="1"/>
+      <c r="B51" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="C51" s="1" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>36</v>
@@ -1827,13 +1855,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="n">
         <v>51</v>
       </c>
-      <c r="B52" s="1"/>
+      <c r="B52" s="1" t="s">
+        <v>108</v>
+      </c>
       <c r="C52" s="1" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>36</v>
@@ -1842,13 +1872,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="n">
         <v>52</v>
       </c>
-      <c r="B53" s="1"/>
+      <c r="B53" s="1" t="s">
+        <v>110</v>
+      </c>
       <c r="C53" s="1" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>36</v>
@@ -1862,10 +1894,10 @@
         <v>53</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>36</v>
@@ -1874,12 +1906,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="n">
         <v>54</v>
       </c>
+      <c r="B55" s="0" t="s">
+        <v>114</v>
+      </c>
       <c r="C55" s="1" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>36</v>
@@ -1888,12 +1923,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="n">
         <v>55</v>
       </c>
+      <c r="B56" s="0" t="s">
+        <v>116</v>
+      </c>
       <c r="C56" s="1" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>36</v>
@@ -1902,12 +1940,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="n">
         <v>56</v>
       </c>
+      <c r="B57" s="0" t="s">
+        <v>118</v>
+      </c>
       <c r="C57" s="1" t="s">
-        <v>112</v>
+        <v>119</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>36</v>
@@ -1921,10 +1962,10 @@
         <v>57</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>113</v>
+        <v>120</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>114</v>
+        <v>121</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>36</v>
@@ -1938,10 +1979,10 @@
         <v>58</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>116</v>
+        <v>123</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>36</v>
@@ -1958,7 +1999,7 @@
         <v>39</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>117</v>
+        <v>124</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>36</v>
@@ -1975,7 +2016,7 @@
         <v>94</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>118</v>
+        <v>125</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>36</v>
@@ -1989,10 +2030,10 @@
         <v>61</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>119</v>
+        <v>126</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>36</v>
@@ -2006,13 +2047,13 @@
         <v>62</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>121</v>
+        <v>128</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>122</v>
+        <v>129</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>123</v>
+        <v>130</v>
       </c>
       <c r="E63" s="5"/>
       <c r="F63" s="1" t="n">
@@ -2044,13 +2085,13 @@
         <v>63</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>125</v>
+        <v>132</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>123</v>
+        <v>130</v>
       </c>
       <c r="F64" s="1" t="n">
         <v>1</v>
@@ -2061,13 +2102,13 @@
         <v>64</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>126</v>
+        <v>133</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>127</v>
+        <v>134</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>123</v>
+        <v>130</v>
       </c>
       <c r="F65" s="1" t="n">
         <v>1</v>
@@ -2078,13 +2119,13 @@
         <v>65</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>128</v>
+        <v>135</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>129</v>
+        <v>136</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>123</v>
+        <v>130</v>
       </c>
       <c r="F66" s="1" t="n">
         <v>1</v>
@@ -2095,13 +2136,13 @@
         <v>66</v>
       </c>
       <c r="B67" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="D67" s="1" t="s">
         <v>130</v>
-      </c>
-      <c r="C67" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="D67" s="1" t="s">
-        <v>123</v>
       </c>
       <c r="F67" s="1" t="n">
         <v>1</v>
@@ -2112,13 +2153,13 @@
         <v>67</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>132</v>
+        <v>139</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>133</v>
+        <v>140</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>123</v>
+        <v>130</v>
       </c>
       <c r="F68" s="1" t="n">
         <v>1</v>
@@ -2129,13 +2170,13 @@
         <v>68</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>134</v>
+        <v>141</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>135</v>
+        <v>142</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>123</v>
+        <v>130</v>
       </c>
       <c r="F69" s="1" t="n">
         <v>1</v>
@@ -2146,13 +2187,13 @@
         <v>69</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>136</v>
+        <v>143</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>137</v>
+        <v>144</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>138</v>
+        <v>145</v>
       </c>
       <c r="E70" s="5"/>
       <c r="F70" s="1" t="n">
@@ -2184,13 +2225,13 @@
         <v>70</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>138</v>
+        <v>145</v>
       </c>
       <c r="F71" s="1" t="n">
         <v>1</v>
@@ -2201,13 +2242,13 @@
         <v>71</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>141</v>
+        <v>148</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>142</v>
+        <v>149</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>138</v>
+        <v>145</v>
       </c>
       <c r="F72" s="1" t="n">
         <v>1</v>
@@ -2218,13 +2259,13 @@
         <v>72</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>143</v>
+        <v>150</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>144</v>
+        <v>151</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>138</v>
+        <v>145</v>
       </c>
       <c r="F73" s="1" t="n">
         <v>1</v>
@@ -2235,13 +2276,13 @@
         <v>73</v>
       </c>
       <c r="B74" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D74" s="1" t="s">
         <v>145</v>
-      </c>
-      <c r="C74" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="D74" s="1" t="s">
-        <v>138</v>
       </c>
       <c r="F74" s="1" t="n">
         <v>1</v>
@@ -2252,13 +2293,13 @@
         <v>74</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>138</v>
+        <v>145</v>
       </c>
       <c r="F75" s="1" t="n">
         <v>1</v>
@@ -2269,13 +2310,13 @@
         <v>75</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>150</v>
+        <v>157</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>138</v>
+        <v>145</v>
       </c>
       <c r="F76" s="1" t="n">
         <v>1</v>
@@ -2285,11 +2326,14 @@
       <c r="A77" s="1" t="n">
         <v>76</v>
       </c>
+      <c r="B77" s="0" t="s">
+        <v>158</v>
+      </c>
       <c r="C77" s="1" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>138</v>
+        <v>145</v>
       </c>
       <c r="F77" s="1" t="n">
         <v>1</v>
@@ -2300,13 +2344,13 @@
         <v>77</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
       <c r="E78" s="5"/>
       <c r="F78" s="1" t="n">
@@ -2338,13 +2382,13 @@
         <v>78</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>156</v>
+        <v>164</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
       <c r="F79" s="1" t="n">
         <v>1</v>
@@ -2355,13 +2399,13 @@
         <v>79</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>157</v>
+        <v>165</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>158</v>
+        <v>166</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
       <c r="F80" s="1" t="n">
         <v>1</v>
@@ -2391,23 +2435,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="16.3775510204082"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="18.3571428571429"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>160</v>
+        <v>168</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>161</v>
+        <v>169</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>162</v>
+        <v>170</v>
       </c>
     </row>
   </sheetData>

</xml_diff>